<commit_message>
big update to sheets
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -34461,7 +34461,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -34471,7 +34471,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>ɡ</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
@@ -34575,7 +34575,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -34689,7 +34689,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -34803,7 +34803,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -34917,7 +34917,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -35031,7 +35031,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -35145,7 +35145,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -35259,7 +35259,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>go.ta.ˈsɨ́.gə</t>
+          <t>ɡo.ta.ˈsɨ́.ɡə</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">

</xml_diff>